<commit_message>
Add data from Second round of testing
</commit_message>
<xml_diff>
--- a/bmes301/lab4/data/lab4_specimen_dimensions.xlsx
+++ b/bmes301/lab4/data/lab4_specimen_dimensions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/178c4c426960fab1/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{EF83996A-2640-4E66-A1CE-A826085AFF14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E28BEE55-8DEB-4C26-95A9-1190E5399E81}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{B357125C-262E-4E5A-B24F-686FBA0C5310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A8C6227D-B4E4-4F7A-9EB3-ED3F97FC7C61}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="15">
   <si>
     <t>Group #</t>
   </si>
@@ -68,6 +68,15 @@
     <t>B</t>
   </si>
   <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>measured directly</t>
+  </si>
+  <si>
     <t>Inner: difference between broken and pre broken</t>
   </si>
 </sst>
@@ -75,7 +84,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,13 +106,25 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9BC2E6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -117,8 +138,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4B084"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -148,6 +175,19 @@
       <bottom style="thick">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -182,6 +222,32 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
@@ -190,9 +256,7 @@
       <top style="thin">
         <color rgb="FFCCCCCC"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -205,8 +269,19 @@
       <top style="thin">
         <color rgb="FFCCCCCC"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -214,7 +289,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -230,34 +305,68 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment readingOrder="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment readingOrder="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -564,11 +673,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,7 +688,7 @@
     <col min="4" max="5" width="13" customWidth="1"/>
     <col min="6" max="6" width="15.28515625" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="62.7109375" customWidth="1"/>
+    <col min="8" max="8" width="46.42578125" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -590,7 +699,7 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -611,498 +720,993 @@
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="D2" s="12">
+      <c r="C2" s="7">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D2" s="18">
         <v>6.7</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="19">
         <v>7.5</v>
       </c>
-      <c r="F2" s="13">
+      <c r="F2" s="19">
         <v>4.6500000000000004</v>
       </c>
-      <c r="G2" s="13">
+      <c r="G2" s="19">
         <v>4.8</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="7">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="D3" s="12">
+      <c r="C3" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="D3" s="18">
         <v>7.57</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="19">
         <v>9.73</v>
       </c>
-      <c r="F3" s="13">
+      <c r="F3" s="19">
         <v>5.57</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="19">
         <v>6.53</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
+      <c r="A4" s="15">
+        <v>1</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D4" s="20">
+        <v>8.23</v>
+      </c>
+      <c r="E4" s="21">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="F4" s="21">
+        <v>3.98</v>
+      </c>
+      <c r="G4" s="21">
+        <v>5.2</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="D5" s="20">
+        <v>6.5</v>
+      </c>
+      <c r="E5" s="20">
+        <v>7.97</v>
+      </c>
+      <c r="F5" s="20">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="G5" s="20">
+        <v>4.45</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B6" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="9">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="D4" s="14">
+      <c r="C6" s="12">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D6" s="22">
         <v>7.1</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E6" s="23">
         <v>8.3000000000000007</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F6" s="24">
         <v>3.9</v>
       </c>
-      <c r="G4" s="16">
+      <c r="G6" s="24">
         <v>5.0999999999999996</v>
       </c>
-      <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+      <c r="H6" s="13"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="12">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B7" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="D5" s="17">
+      <c r="C7" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="30">
         <v>6.7</v>
       </c>
-      <c r="E5" s="18">
+      <c r="E7" s="31">
         <v>7.1</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F7" s="24">
         <v>4.0999999999999996</v>
       </c>
-      <c r="G5" s="16">
+      <c r="G7" s="24">
         <v>4.5</v>
       </c>
-      <c r="H5" s="10"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>2</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="27">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D8" s="34">
+        <v>8.6</v>
+      </c>
+      <c r="E8" s="34">
+        <v>9.9</v>
+      </c>
+      <c r="F8" s="29">
+        <v>5.33</v>
+      </c>
+      <c r="G8" s="25">
+        <v>6.63</v>
+      </c>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>2</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="28">
+        <v>0.4</v>
+      </c>
+      <c r="D9" s="34">
+        <v>7.1</v>
+      </c>
+      <c r="E9" s="34">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F9" s="29">
+        <v>5.83</v>
+      </c>
+      <c r="G9" s="25">
+        <v>7.03</v>
+      </c>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="D6" s="12">
+      <c r="C10" s="7">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D10" s="32">
         <v>8.84</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E10" s="33">
         <v>12</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F10" s="19">
         <v>7.14</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G10" s="19">
         <v>9.1</v>
       </c>
-      <c r="H6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="H10" s="8"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
         <v>3</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="D7" s="12">
+      <c r="C11" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="D11" s="18">
         <v>9.17</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E11" s="19">
         <v>9.5299999999999994</v>
       </c>
-      <c r="F7" s="13">
+      <c r="F11" s="19">
         <v>5</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G11" s="19">
         <v>5.6</v>
       </c>
-      <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
+      <c r="H11" s="8"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
+        <v>3</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D12" s="20">
+        <v>7.23</v>
+      </c>
+      <c r="E12" s="21">
+        <v>9</v>
+      </c>
+      <c r="F12" s="21">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="G12" s="21">
+        <v>5.2</v>
+      </c>
+      <c r="H12" s="16"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>3</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="D13" s="20">
+        <v>6.2</v>
+      </c>
+      <c r="E13" s="20">
+        <v>7.2</v>
+      </c>
+      <c r="F13" s="20">
+        <v>3.8</v>
+      </c>
+      <c r="G13" s="20">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="H13" s="16"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>4</v>
+      </c>
+      <c r="B14" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="9">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="D8" s="16">
+      <c r="C14" s="12">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D14" s="24">
         <v>9.75</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E14" s="24">
         <v>10.9</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F14" s="24">
         <v>6.758</v>
       </c>
-      <c r="G8" s="16">
+      <c r="G14" s="24">
         <v>7.47</v>
       </c>
-      <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="12">
         <v>4</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="D9" s="16">
+      <c r="C15" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="D15" s="24">
         <v>9.23</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E15" s="24">
         <v>11.67</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F15" s="24">
         <v>6.1</v>
       </c>
-      <c r="G9" s="16">
+      <c r="G15" s="24">
         <v>7.97</v>
       </c>
-      <c r="H9" s="10"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>4</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D16" s="25">
+        <v>8</v>
+      </c>
+      <c r="E16" s="25">
+        <v>8.9</v>
+      </c>
+      <c r="F16" s="25">
+        <v>5.5</v>
+      </c>
+      <c r="G16" s="25">
+        <v>6.23</v>
+      </c>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>4</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D17" s="26">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="E17" s="26">
+        <v>10.8</v>
+      </c>
+      <c r="F17" s="25">
+        <v>5.94</v>
+      </c>
+      <c r="G17" s="25">
+        <v>6.97</v>
+      </c>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
         <v>5</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="5">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="D10" s="12">
+      <c r="C18" s="7">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D18" s="18">
         <v>8.5</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E18" s="19">
         <v>10</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F18" s="19">
         <v>5.0999999999999996</v>
       </c>
-      <c r="G10" s="13">
+      <c r="G18" s="19">
         <v>6.4</v>
       </c>
-      <c r="H10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
+      <c r="H18" s="8"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
         <v>5</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B19" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="D11" s="12">
+      <c r="C19" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="D19" s="18">
         <v>8.6</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E19" s="19">
         <v>10.3</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F19" s="19">
         <v>5.5</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G19" s="19">
         <v>6.5</v>
       </c>
-      <c r="H11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
+      <c r="H19" s="8"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>5</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D20" s="20">
+        <v>7.3</v>
+      </c>
+      <c r="E20" s="21">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F20" s="21">
+        <f>7.3-1.9*2</f>
+        <v>3.5</v>
+      </c>
+      <c r="G20" s="21">
+        <v>5.9</v>
+      </c>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>5</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="D21" s="20">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E21" s="20">
+        <v>10.7</v>
+      </c>
+      <c r="F21" s="20">
+        <f>8.3-1.7*2</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="G21" s="20">
+        <v>7.5</v>
+      </c>
+      <c r="H21" s="16"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="12">
         <v>6</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B22" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="9">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="D12" s="16">
+      <c r="C22" s="12">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D22" s="24">
         <v>8.3000000000000007</v>
       </c>
-      <c r="E12" s="16">
+      <c r="E22" s="24">
         <v>10.199999999999999</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F22" s="24">
         <v>6.33</v>
       </c>
-      <c r="G12" s="16">
+      <c r="G22" s="24">
         <v>8.23</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H22" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="12">
+        <v>6</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="D23" s="24">
+        <v>8.33</v>
+      </c>
+      <c r="E23" s="24">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="F23" s="24">
+        <v>7.3</v>
+      </c>
+      <c r="G23" s="24">
+        <v>7.5</v>
+      </c>
+      <c r="H23" s="13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>6</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
+      <c r="C24" s="5">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D24" s="25">
+        <v>8.23</v>
+      </c>
+      <c r="E24" s="25">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F24" s="25">
+        <f>D24-1.7</f>
+        <v>6.53</v>
+      </c>
+      <c r="G24" s="25">
+        <f>E24-1.7</f>
+        <v>7.1000000000000005</v>
+      </c>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
         <v>6</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D25" s="26">
+        <v>11.1</v>
+      </c>
+      <c r="E25" s="26">
+        <v>13.7</v>
+      </c>
+      <c r="F25" s="25">
+        <f>D25-1.83</f>
+        <v>9.27</v>
+      </c>
+      <c r="G25" s="25">
+        <f>E25-1.83</f>
+        <v>11.87</v>
+      </c>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>7</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D26" s="18">
+        <v>6.9</v>
+      </c>
+      <c r="E26" s="19">
+        <v>7.3</v>
+      </c>
+      <c r="F26" s="19">
+        <v>3.8</v>
+      </c>
+      <c r="G26" s="19">
+        <v>4.2</v>
+      </c>
+      <c r="H26" s="8"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>7</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="D13" s="16">
-        <v>8.33</v>
-      </c>
-      <c r="E13" s="16">
-        <v>8.5299999999999994</v>
-      </c>
-      <c r="F13" s="16">
-        <v>7.3</v>
-      </c>
-      <c r="G13" s="16">
-        <v>7.5</v>
-      </c>
-      <c r="H13" s="10" t="s">
+      <c r="C27" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="D27" s="18">
+        <v>8.9</v>
+      </c>
+      <c r="E27" s="19">
+        <v>11.2</v>
+      </c>
+      <c r="F27" s="19">
+        <v>5.6</v>
+      </c>
+      <c r="G27" s="19">
+        <v>6.7</v>
+      </c>
+      <c r="H27" s="8"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>7</v>
+      </c>
+      <c r="B28" s="15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+      <c r="C28" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D28" s="20">
+        <v>8</v>
+      </c>
+      <c r="E28" s="21">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F28" s="21">
+        <v>4.7</v>
+      </c>
+      <c r="G28" s="21">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H28" s="16"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
         <v>7</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B29" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="D29" s="20">
+        <v>7.2</v>
+      </c>
+      <c r="E29" s="20">
+        <v>9</v>
+      </c>
+      <c r="F29" s="20">
+        <v>5</v>
+      </c>
+      <c r="G29" s="20">
+        <v>5.5</v>
+      </c>
+      <c r="H29" s="16"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="12">
         <v>8</v>
       </c>
-      <c r="C14" s="5">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="D14" s="12">
-        <v>6.9</v>
-      </c>
-      <c r="E14" s="13">
-        <v>7.3</v>
-      </c>
-      <c r="F14" s="13">
-        <v>3.8</v>
-      </c>
-      <c r="G14" s="13">
-        <v>4.2</v>
-      </c>
-      <c r="H14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>7</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="D15" s="12">
-        <v>8.9</v>
-      </c>
-      <c r="E15" s="13">
-        <v>11.2</v>
-      </c>
-      <c r="F15" s="13">
-        <v>5.6</v>
-      </c>
-      <c r="G15" s="13">
-        <v>6.7</v>
-      </c>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+      <c r="B30" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="9">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="D16" s="16">
+      <c r="C30" s="12">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D30" s="24">
         <f>AVERAGE(7.5,9.4,7.7,8.4,7.8)</f>
         <v>8.16</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E30" s="24">
         <f>AVERAGE(8.1,11.1,9.8,8.7,8)</f>
         <v>9.14</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F30" s="24">
         <f>8.16-0.8-1.3</f>
         <v>6.0600000000000005</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G30" s="24">
         <f>9.14-0.6-0.8</f>
         <v>7.7400000000000011</v>
       </c>
-      <c r="H16" s="10"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="12">
         <v>8</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B31" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="D17" s="16">
+      <c r="C31" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="D31" s="24">
         <f>AVERAGE(6.7,7.3,8.8,8.1,6.6)</f>
         <v>7.5</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E31" s="24">
         <f>AVERAGE(7.5,8.8,9.6,8.2,7.7)</f>
         <v>8.36</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F31" s="24">
         <v>4.05</v>
       </c>
-      <c r="G17" s="16">
+      <c r="G31" s="24">
         <v>4.2</v>
       </c>
-      <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>8</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="5">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D32" s="25">
+        <f>AVERAGE(7.2,6.7,8.3,7.6,6.7)</f>
+        <v>7.3000000000000016</v>
+      </c>
+      <c r="E32" s="25">
+        <f>AVERAGE(7.3,10,9.4,8,7.8)</f>
+        <v>8.5</v>
+      </c>
+      <c r="F32" s="25">
+        <v>3.85</v>
+      </c>
+      <c r="G32" s="25">
+        <v>4.55</v>
+      </c>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>8</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D33" s="26">
+        <f>AVERAGE(7.8,8,9.2,8,7.5)</f>
+        <v>8.1</v>
+      </c>
+      <c r="E33" s="26">
+        <f>AVERAGE(10.1,8.1,9.4,8.2,8.7)</f>
+        <v>8.9</v>
+      </c>
+      <c r="F33" s="25">
+        <v>5.65</v>
+      </c>
+      <c r="G33" s="25">
+        <f>AVERAGE(5.3,6.1)</f>
+        <v>5.6999999999999993</v>
+      </c>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
         <v>9</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B34" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="5">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="D18" s="12">
+      <c r="C34" s="7">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D34" s="18">
         <v>7.93</v>
       </c>
-      <c r="E18" s="13">
+      <c r="E34" s="19">
         <v>8.67</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F34" s="19">
         <v>3.4</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G34" s="19">
         <v>4.3</v>
       </c>
-      <c r="H18" s="6"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+      <c r="H34" s="8"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
         <v>9</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B35" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="D19" s="12">
+      <c r="C35" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="D35" s="18">
         <v>7.87</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E35" s="19">
         <v>8.73</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F35" s="19">
         <v>4.3</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G35" s="19">
         <v>4.5</v>
       </c>
-      <c r="H19" s="6"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="9">
+      <c r="H35" s="8"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
+        <v>9</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="15">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D36" s="20">
+        <v>6.63</v>
+      </c>
+      <c r="E36" s="21">
+        <v>7.16</v>
+      </c>
+      <c r="F36" s="21">
+        <v>4.63</v>
+      </c>
+      <c r="G36" s="21">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="H36" s="16"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
+        <v>9</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C37" s="17">
+        <v>0.4</v>
+      </c>
+      <c r="D37" s="20">
+        <v>7.5</v>
+      </c>
+      <c r="E37" s="20">
+        <v>8.73</v>
+      </c>
+      <c r="F37" s="20">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="G37" s="20">
+        <v>5.7</v>
+      </c>
+      <c r="H37" s="16"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
         <v>10</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B38" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C20" s="9">
-        <v>1.6000000000000001E-3</v>
-      </c>
-      <c r="D20" s="16">
+      <c r="C38" s="12">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D38" s="24">
         <v>7.3666666669999996</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E38" s="24">
         <v>8.8666666670000005</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F38" s="24">
         <v>4.5666666669999998</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G38" s="24">
         <v>5.9666666670000001</v>
       </c>
-      <c r="H20" s="10"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
         <v>10</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B39" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="11">
-        <v>0.4</v>
-      </c>
-      <c r="D21" s="16">
+      <c r="C39" s="14">
+        <v>0.4</v>
+      </c>
+      <c r="D39" s="24">
         <v>10.03333333</v>
       </c>
-      <c r="E21" s="16">
+      <c r="E39" s="24">
         <v>11.06666667</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F39" s="24">
         <v>8.2333333329999991</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G39" s="24">
         <v>8.1166666670000005</v>
       </c>
-      <c r="H21" s="10"/>
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="5">
+        <v>10</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="5">
+        <v>1.6000000000000001E-3</v>
+      </c>
+      <c r="D40" s="25">
+        <v>6.1</v>
+      </c>
+      <c r="E40" s="25">
+        <v>7.1</v>
+      </c>
+      <c r="F40" s="25">
+        <v>3.86</v>
+      </c>
+      <c r="G40" s="25">
+        <v>4</v>
+      </c>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
+        <v>10</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C41" s="11">
+        <v>0.4</v>
+      </c>
+      <c r="D41" s="26">
+        <v>7.4</v>
+      </c>
+      <c r="E41" s="26">
+        <v>7.76</v>
+      </c>
+      <c r="F41" s="25">
+        <v>4.7300000000000004</v>
+      </c>
+      <c r="G41" s="25">
+        <v>4.43</v>
+      </c>
+      <c r="H41" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>